<commit_message>
more stuff to cv
</commit_message>
<xml_diff>
--- a/wintersmith/data/cv.xlsx
+++ b/wintersmith/data/cv.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14480" yWindow="2080" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="23200" yWindow="9780" windowWidth="25600" windowHeight="18380" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="publications" sheetId="1" r:id="rId1"/>
     <sheet name="service" sheetId="2" r:id="rId2"/>
     <sheet name="grants" sheetId="3" r:id="rId3"/>
     <sheet name="awards" sheetId="4" r:id="rId4"/>
+    <sheet name="teaching" sheetId="5" r:id="rId5"/>
+    <sheet name="education" sheetId="6" r:id="rId6"/>
+    <sheet name="phd" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="166">
   <si>
     <t>IDC</t>
   </si>
@@ -280,6 +283,246 @@
   </si>
   <si>
     <t>venueFull</t>
+  </si>
+  <si>
+    <t>course</t>
+  </si>
+  <si>
+    <t>HCC Big Data</t>
+  </si>
+  <si>
+    <t>Rapid Prototyping</t>
+  </si>
+  <si>
+    <t>instructor</t>
+  </si>
+  <si>
+    <t>committee member</t>
+  </si>
+  <si>
+    <t>senior thesis</t>
+  </si>
+  <si>
+    <t>student</t>
+  </si>
+  <si>
+    <t>Homa Hosseinmardi</t>
+  </si>
+  <si>
+    <t>Mahnaz Roshanaei</t>
+  </si>
+  <si>
+    <t>Study and Analysis of Emotions in Online Social Networks and Smartphones</t>
+  </si>
+  <si>
+    <t>Characterization of User Behavior in Social Networks to Better Understand Cyberbullying</t>
+  </si>
+  <si>
+    <t>Cognitive Demand of Engineering Information</t>
+  </si>
+  <si>
+    <t>PhD thesis proposal</t>
+  </si>
+  <si>
+    <t>John Brendan Sweany</t>
+  </si>
+  <si>
+    <t>MS thesis defense</t>
+  </si>
+  <si>
+    <t>advisor</t>
+  </si>
+  <si>
+    <t>Michael Aaron</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Emily Bertelson</t>
+  </si>
+  <si>
+    <t>Ross Michael Holland</t>
+  </si>
+  <si>
+    <t>Applications of Graph Technology to Digital Content Recommendation</t>
+  </si>
+  <si>
+    <t>Devon Tivona</t>
+  </si>
+  <si>
+    <t>Redhwan Nour</t>
+  </si>
+  <si>
+    <t>PhD prelim</t>
+  </si>
+  <si>
+    <t>User-Centered Design and Development II</t>
+  </si>
+  <si>
+    <t>Erik Komendera</t>
+  </si>
+  <si>
+    <t>PhD thesis defense</t>
+  </si>
+  <si>
+    <t>Precise Assembly of Truss Structures by Distributed Robots</t>
+  </si>
+  <si>
+    <t>Kelvin Andrew Kosbab</t>
+  </si>
+  <si>
+    <t>Crowd Dynamics of Athletic Events</t>
+  </si>
+  <si>
+    <t>Jeff Hoehl</t>
+  </si>
+  <si>
+    <t>Simplifying the Web Experience for People with Cognitive Disabilities</t>
+  </si>
+  <si>
+    <t>Web accessibility for Cognition</t>
+  </si>
+  <si>
+    <t>Thomas Michael Erickson</t>
+  </si>
+  <si>
+    <t>independent study</t>
+  </si>
+  <si>
+    <t>Integrating Arduino with 3D-printed Tactile Picture Books</t>
+  </si>
+  <si>
+    <t>MS thesis</t>
+  </si>
+  <si>
+    <t>Esther Vasiete Allas</t>
+  </si>
+  <si>
+    <t>Multimodal frustration detection on smartphones</t>
+  </si>
+  <si>
+    <t>Dara Cunningham</t>
+  </si>
+  <si>
+    <t>Building inhabitant feedback: Creating a reflective practice for environmental design using activity theory</t>
+  </si>
+  <si>
+    <t>Health Craft: Towards Helping Children Craft Personal Health Technologies</t>
+  </si>
+  <si>
+    <t>Swamy Ananthanarayan</t>
+  </si>
+  <si>
+    <t>Kyu Han Koh</t>
+  </si>
+  <si>
+    <t>Computational Thinking Pattern Analysis: A Phenomenological Approach To Compute Computational Thinking</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>PostDoc</t>
+  </si>
+  <si>
+    <t>PhD Computer Science</t>
+  </si>
+  <si>
+    <t>MS Computer Science</t>
+  </si>
+  <si>
+    <t>Simon Fraser University</t>
+  </si>
+  <si>
+    <t>org</t>
+  </si>
+  <si>
+    <t>University of Maryland College Park</t>
+  </si>
+  <si>
+    <t>MIT</t>
+  </si>
+  <si>
+    <t>BSc Computer Science</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>Burnaby</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>College Park</t>
+  </si>
+  <si>
+    <t>The Student Affairs Faculty of the Year Award recognizes a superb faculty member that demonstrates outstanding engagement with students and contributions to the university community based on areas such as promoting diversity or fostering intellectual growth.</t>
+  </si>
+  <si>
+    <t>Khalid Alharbi</t>
+  </si>
+  <si>
+    <t>Abigale Stangl</t>
+  </si>
+  <si>
+    <t>department</t>
+  </si>
+  <si>
+    <t>Computer Science</t>
+  </si>
+  <si>
+    <t>ATLAS</t>
+  </si>
+  <si>
+    <t>Jackie Cameron</t>
+  </si>
+  <si>
+    <t>Jeeeun Kim</t>
+  </si>
+  <si>
+    <t>Mike Skirpan</t>
+  </si>
+  <si>
+    <t>Layne Hubbard</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>course work</t>
+  </si>
+  <si>
+    <t>proposal</t>
+  </si>
+  <si>
+    <t>incoming</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>Graduate Committee</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>Faculty Search Committee</t>
+  </si>
+  <si>
+    <t>organization</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>ATLAS Mini-Grant</t>
+  </si>
+  <si>
+    <t>Data Science for Social Good: Hackathons and Public Exhibits to Engage Students and Increase Campus Awareness</t>
   </si>
 </sst>
 </file>
@@ -328,7 +571,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -372,11 +615,96 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="125">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -398,6 +726,47 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -419,6 +788,47 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -750,8 +1160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -785,33 +1195,33 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -825,16 +1235,13 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -842,16 +1249,16 @@
         <v>2014</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -859,16 +1266,19 @@
         <v>2014</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -876,16 +1286,16 @@
         <v>2014</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -893,16 +1303,16 @@
         <v>2014</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -910,16 +1320,16 @@
         <v>2014</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -927,16 +1337,16 @@
         <v>2014</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -944,13 +1354,13 @@
         <v>2014</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
         <v>21</v>
@@ -961,19 +1371,16 @@
         <v>2014</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -981,58 +1388,61 @@
         <v>2014</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D14" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s">
         <v>11</v>
       </c>
+      <c r="F14" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:F15">
-    <sortCondition ref="A1"/>
+    <sortCondition descending="1" ref="A1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1046,15 +1456,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>78</v>
       </c>
@@ -1062,10 +1472,13 @@
         <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>162</v>
+      </c>
+      <c r="D1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>2014</v>
       </c>
@@ -1076,30 +1489,81 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2014</v>
       </c>
       <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>2014</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>2014</v>
+      </c>
+      <c r="B5" t="s">
         <v>48</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>2014</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6" t="s">
         <v>48</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>2014</v>
+      </c>
+      <c r="B7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C7" t="s">
+        <v>158</v>
+      </c>
+      <c r="D7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>2014</v>
+      </c>
+      <c r="B8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D8" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1110,10 +1574,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1287,39 +1751,39 @@
         <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>165</v>
       </c>
       <c r="C9" t="s">
         <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>164</v>
       </c>
       <c r="E9">
-        <v>2012</v>
+        <v>2014</v>
       </c>
       <c r="F9">
-        <v>2013</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E10">
         <v>2012</v>
       </c>
       <c r="F10">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1327,18 +1791,38 @@
         <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E11">
         <v>2012</v>
       </c>
       <c r="F11">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12">
+        <v>2012</v>
+      </c>
+      <c r="F12">
         <v>2014</v>
       </c>
     </row>
@@ -1357,7 +1841,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1388,9 +1874,611 @@
       <c r="C2" t="s">
         <v>60</v>
       </c>
+      <c r="D2" t="s">
+        <v>144</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>2015</v>
+      </c>
+      <c r="B2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>2015</v>
+      </c>
+      <c r="B3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>2015</v>
+      </c>
+      <c r="B4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>2015</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>2014</v>
+      </c>
+      <c r="B7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>2014</v>
+      </c>
+      <c r="B8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>2014</v>
+      </c>
+      <c r="B9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>2014</v>
+      </c>
+      <c r="B10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>2014</v>
+      </c>
+      <c r="B11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>2014</v>
+      </c>
+      <c r="B12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>2014</v>
+      </c>
+      <c r="B13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>2014</v>
+      </c>
+      <c r="B14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>2014</v>
+      </c>
+      <c r="B15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>2014</v>
+      </c>
+      <c r="B16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>2014</v>
+      </c>
+      <c r="B17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" t="s">
+        <v>124</v>
+      </c>
+      <c r="D17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>2014</v>
+      </c>
+      <c r="B18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>2014</v>
+      </c>
+      <c r="B19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" t="s">
+        <v>127</v>
+      </c>
+      <c r="D19" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>2014</v>
+      </c>
+      <c r="B20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D20" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:E18">
+    <sortCondition descending="1" ref="A1"/>
+  </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>2009</v>
+      </c>
+      <c r="B2">
+        <v>2012</v>
+      </c>
+      <c r="C2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>2005</v>
+      </c>
+      <c r="B3">
+        <v>2009</v>
+      </c>
+      <c r="C3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>2003</v>
+      </c>
+      <c r="B4">
+        <v>2005</v>
+      </c>
+      <c r="C4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>1997</v>
+      </c>
+      <c r="B5">
+        <v>2001</v>
+      </c>
+      <c r="C5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>2013</v>
+      </c>
+      <c r="B2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>2013</v>
+      </c>
+      <c r="B3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>2013</v>
+      </c>
+      <c r="B4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>2014</v>
+      </c>
+      <c r="B5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>2015</v>
+      </c>
+      <c r="B7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" t="s">
+        <v>148</v>
+      </c>
+      <c r="D7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>